<commit_message>
Added an Excel Graph, corrected some minor mistakes.
</commit_message>
<xml_diff>
--- a/Simulationen.xlsx
+++ b/Simulationen.xlsx
@@ -125,8 +125,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Ausfallwahrscheinlichkeit</a:t>
+              <a:t>Vergleich</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> der Ausfallwahrscheinlichkeiten</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -169,6 +174,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>redundancy, with repair</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -816,6 +824,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>no redundancy</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
@@ -826,7 +837,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -1466,6 +1477,654 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Redundancy, no repair</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$V$3:$V$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>110000.00000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>114999.99999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>135000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>165000</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>175000</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>185000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>195000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>204999.99999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>210000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>215000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>220000.00000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>225000</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>229999.99999999997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>235000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>240000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>245000.00000000003</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>254999.99999999997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>260000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>265000</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>270000</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>275000</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>280000</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>285000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>290000</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>295000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>305000</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>310000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>315000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>320000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>325000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>330000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>335000</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>340000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>345000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>350000</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>355000</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>360000</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>365000</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>370000</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>375000</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>380000</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>385000</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>390000</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>395000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>405000</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>409999.99999999994</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>415000.00000000006</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>420000</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>425000</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>430000</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>434999.99999999994</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>440000.00000000006</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>445000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>450000</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>455000</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>459999.99999999994</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>465000.00000000006</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>470000</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>475000</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>480000</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>484999.99999999994</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>490000.00000000006</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>495000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$W$3:$W$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51788999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86053999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96548999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99206000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99825000000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99962000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99992000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99998000000000009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1474,11 +2133,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="420997984"/>
-        <c:axId val="420991320"/>
+        <c:axId val="364140584"/>
+        <c:axId val="364143328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="420997984"/>
+        <c:axId val="364140584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1498,8 +2157,78 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>time t</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1535,12 +2264,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420991320"/>
+        <c:crossAx val="364143328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="420991320"/>
+        <c:axId val="364143328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,8 +2289,78 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Probability of fail</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1597,7 +2396,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420997984"/>
+        <c:crossAx val="364140584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1609,6 +2408,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2207,15 +3038,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>119061</xdr:rowOff>
+      <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2500,10 +3331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O102"/>
+  <dimension ref="A1:W102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,7 +3343,7 @@
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>2</v>
       </c>
@@ -2526,7 +3357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2568,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2609,8 +3440,28 @@
         <f t="shared" ref="O3:O66" si="3">K3*10^(L3)</f>
         <v>0.27385000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>Q3*10^(R3)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>S3*10^(T3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2651,8 +3502,28 @@
         <f t="shared" si="3"/>
         <v>0.47271000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>5.1788999999999996</v>
+      </c>
+      <c r="T4">
+        <v>-1</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ref="V4:V67" si="4">Q4*10^(R4)</f>
+        <v>5000</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ref="W4:W67" si="5">S4*10^(T4)</f>
+        <v>0.51788999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -2693,8 +3564,28 @@
         <f t="shared" si="3"/>
         <v>0.61711000000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>8.6053999999999995</v>
+      </c>
+      <c r="T5">
+        <v>-1</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="5"/>
+        <v>0.86053999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2735,8 +3626,28 @@
         <f t="shared" si="3"/>
         <v>0.72196000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>1.5</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>9.6548999999999996</v>
+      </c>
+      <c r="T6">
+        <v>-1</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="4"/>
+        <v>15000</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="5"/>
+        <v>0.96548999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -2777,8 +3688,28 @@
         <f t="shared" si="3"/>
         <v>0.79810000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>9.9206000000000003</v>
+      </c>
+      <c r="T7">
+        <v>-1</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="4"/>
+        <v>20000</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="5"/>
+        <v>0.99206000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2819,8 +3750,28 @@
         <f t="shared" si="3"/>
         <v>0.85338999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>2.5</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>9.9824999999999999</v>
+      </c>
+      <c r="T8">
+        <v>-1</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="4"/>
+        <v>25000</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="5"/>
+        <v>0.99825000000000008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -2861,8 +3812,28 @@
         <f t="shared" si="3"/>
         <v>0.89354</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9">
+        <v>9.9962</v>
+      </c>
+      <c r="T9">
+        <v>-1</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="4"/>
+        <v>30000</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="5"/>
+        <v>0.99962000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2903,8 +3874,28 @@
         <f t="shared" si="3"/>
         <v>0.92270000000000008</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>3.5</v>
+      </c>
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>9.9992000000000001</v>
+      </c>
+      <c r="T10">
+        <v>-1</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="4"/>
+        <v>35000</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="5"/>
+        <v>0.99992000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4.5</v>
       </c>
@@ -2945,8 +3936,28 @@
         <f t="shared" si="3"/>
         <v>0.9438700000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>9.9998000000000005</v>
+      </c>
+      <c r="T11">
+        <v>-1</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="4"/>
+        <v>40000</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="5"/>
+        <v>0.99998000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2987,8 +3998,28 @@
         <f t="shared" si="3"/>
         <v>0.95923999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>4.5</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="4"/>
+        <v>45000</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -3029,8 +4060,28 @@
         <f t="shared" si="3"/>
         <v>0.97040000000000015</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="4"/>
+        <v>50000</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3071,8 +4122,28 @@
         <f t="shared" si="3"/>
         <v>0.97850999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>5.5</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="4"/>
+        <v>55000</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6.5</v>
       </c>
@@ -3113,8 +4184,28 @@
         <f t="shared" si="3"/>
         <v>0.98438999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>6</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="4"/>
+        <v>60000</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -3155,8 +4246,28 @@
         <f t="shared" si="3"/>
         <v>0.98866999999999994</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>6.5</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="4"/>
+        <v>65000</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.5</v>
       </c>
@@ -3197,8 +4308,28 @@
         <f t="shared" si="3"/>
         <v>0.99177000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>7</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="4"/>
+        <v>70000</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -3239,8 +4370,28 @@
         <f t="shared" si="3"/>
         <v>0.99402000000000013</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>7.5</v>
+      </c>
+      <c r="R18">
+        <v>4</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="4"/>
+        <v>75000</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8.5</v>
       </c>
@@ -3281,8 +4432,28 @@
         <f t="shared" si="3"/>
         <v>0.99565999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>8</v>
+      </c>
+      <c r="R19">
+        <v>4</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="4"/>
+        <v>80000</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -3323,8 +4494,28 @@
         <f t="shared" si="3"/>
         <v>0.99685000000000012</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>8.5</v>
+      </c>
+      <c r="R20">
+        <v>4</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="4"/>
+        <v>85000</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9.5</v>
       </c>
@@ -3365,8 +4556,28 @@
         <f t="shared" si="3"/>
         <v>0.9977100000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>9</v>
+      </c>
+      <c r="R21">
+        <v>4</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="4"/>
+        <v>90000</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3407,8 +4618,28 @@
         <f t="shared" si="3"/>
         <v>0.99834000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>9.5</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="4"/>
+        <v>95000</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.05</v>
       </c>
@@ -3449,8 +4680,28 @@
         <f t="shared" si="3"/>
         <v>0.99879000000000007</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="4"/>
+        <v>100000</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.1000000000000001</v>
       </c>
@@ -3491,8 +4742,28 @@
         <f t="shared" si="3"/>
         <v>0.99912000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>1.05</v>
+      </c>
+      <c r="R24">
+        <v>5</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="4"/>
+        <v>105000</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.1499999999999999</v>
       </c>
@@ -3533,8 +4804,28 @@
         <f t="shared" si="3"/>
         <v>0.99936000000000014</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R25">
+        <v>5</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="4"/>
+        <v>110000.00000000001</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1.2</v>
       </c>
@@ -3575,8 +4866,28 @@
         <f t="shared" si="3"/>
         <v>0.9995400000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R26">
+        <v>5</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="4"/>
+        <v>114999.99999999999</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1.25</v>
       </c>
@@ -3617,8 +4928,28 @@
         <f t="shared" si="3"/>
         <v>0.9996600000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>1.2</v>
+      </c>
+      <c r="R27">
+        <v>5</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="4"/>
+        <v>120000</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1.3</v>
       </c>
@@ -3659,8 +4990,28 @@
         <f t="shared" si="3"/>
         <v>0.99976000000000009</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>1.25</v>
+      </c>
+      <c r="R28">
+        <v>5</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="4"/>
+        <v>125000</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1.35</v>
       </c>
@@ -3701,8 +5052,28 @@
         <f t="shared" si="3"/>
         <v>0.99982000000000015</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>1.3</v>
+      </c>
+      <c r="R29">
+        <v>5</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="4"/>
+        <v>130000</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1.4</v>
       </c>
@@ -3743,8 +5114,28 @@
         <f t="shared" si="3"/>
         <v>0.99987000000000004</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>1.35</v>
+      </c>
+      <c r="R30">
+        <v>5</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="4"/>
+        <v>135000</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1.45</v>
       </c>
@@ -3785,8 +5176,28 @@
         <f t="shared" si="3"/>
         <v>0.99991000000000008</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>1.4</v>
+      </c>
+      <c r="R31">
+        <v>5</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="4"/>
+        <v>140000</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1.5</v>
       </c>
@@ -3827,8 +5238,28 @@
         <f t="shared" si="3"/>
         <v>0.99992999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>1.45</v>
+      </c>
+      <c r="R32">
+        <v>5</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="4"/>
+        <v>145000</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1.55</v>
       </c>
@@ -3869,8 +5300,28 @@
         <f t="shared" si="3"/>
         <v>0.99995000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>1.5</v>
+      </c>
+      <c r="R33">
+        <v>5</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="4"/>
+        <v>150000</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1.6</v>
       </c>
@@ -3911,8 +5362,28 @@
         <f t="shared" si="3"/>
         <v>0.99995999999999996</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>1.55</v>
+      </c>
+      <c r="R34">
+        <v>5</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="4"/>
+        <v>155000</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1.65</v>
       </c>
@@ -3953,8 +5424,28 @@
         <f t="shared" si="3"/>
         <v>0.99997000000000014</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>1.6</v>
+      </c>
+      <c r="R35">
+        <v>5</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="4"/>
+        <v>160000</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1.7</v>
       </c>
@@ -3995,8 +5486,28 @@
         <f t="shared" si="3"/>
         <v>0.99998000000000009</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>1.65</v>
+      </c>
+      <c r="R36">
+        <v>5</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="4"/>
+        <v>165000</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.75</v>
       </c>
@@ -4037,8 +5548,28 @@
         <f t="shared" si="3"/>
         <v>0.99999000000000005</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>1.7</v>
+      </c>
+      <c r="R37">
+        <v>5</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="4"/>
+        <v>170000</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1.8</v>
       </c>
@@ -4079,8 +5610,28 @@
         <f t="shared" si="3"/>
         <v>0.99999000000000005</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>1.75</v>
+      </c>
+      <c r="R38">
+        <v>5</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="4"/>
+        <v>175000</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1.85</v>
       </c>
@@ -4121,8 +5672,28 @@
         <f t="shared" si="3"/>
         <v>0.99999000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>1.8</v>
+      </c>
+      <c r="R39">
+        <v>5</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="4"/>
+        <v>180000</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1.9</v>
       </c>
@@ -4163,8 +5734,28 @@
         <f t="shared" si="3"/>
         <v>0.99999000000000005</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>1.85</v>
+      </c>
+      <c r="R40">
+        <v>5</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="4"/>
+        <v>185000</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1.95</v>
       </c>
@@ -4205,8 +5796,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>1.9</v>
+      </c>
+      <c r="R41">
+        <v>5</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="4"/>
+        <v>190000</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4247,8 +5858,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>1.95</v>
+      </c>
+      <c r="R42">
+        <v>5</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="4"/>
+        <v>195000</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2.0499999999999998</v>
       </c>
@@ -4289,8 +5920,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>2</v>
+      </c>
+      <c r="R43">
+        <v>5</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2.1</v>
       </c>
@@ -4331,8 +5982,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="R44">
+        <v>5</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="4"/>
+        <v>204999.99999999997</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2.15</v>
       </c>
@@ -4373,8 +6044,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>2.1</v>
+      </c>
+      <c r="R45">
+        <v>5</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="4"/>
+        <v>210000</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2.2000000000000002</v>
       </c>
@@ -4415,8 +6106,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>2.15</v>
+      </c>
+      <c r="R46">
+        <v>5</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="4"/>
+        <v>215000</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2.25</v>
       </c>
@@ -4457,8 +6168,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R47">
+        <v>5</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="4"/>
+        <v>220000.00000000003</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2.2999999999999998</v>
       </c>
@@ -4499,8 +6230,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>2.25</v>
+      </c>
+      <c r="R48">
+        <v>5</v>
+      </c>
+      <c r="S48">
+        <v>1</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="4"/>
+        <v>225000</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2.35</v>
       </c>
@@ -4541,8 +6292,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="R49">
+        <v>5</v>
+      </c>
+      <c r="S49">
+        <v>1</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="4"/>
+        <v>229999.99999999997</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2.4</v>
       </c>
@@ -4583,8 +6354,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>2.35</v>
+      </c>
+      <c r="R50">
+        <v>5</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <f t="shared" si="4"/>
+        <v>235000</v>
+      </c>
+      <c r="W50">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2.4500000000000002</v>
       </c>
@@ -4625,8 +6416,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q51">
+        <v>2.4</v>
+      </c>
+      <c r="R51">
+        <v>5</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <f t="shared" si="4"/>
+        <v>240000</v>
+      </c>
+      <c r="W51">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2.5</v>
       </c>
@@ -4667,8 +6478,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q52">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="R52">
+        <v>5</v>
+      </c>
+      <c r="S52">
+        <v>1</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="V52">
+        <f t="shared" si="4"/>
+        <v>245000.00000000003</v>
+      </c>
+      <c r="W52">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2.5499999999999998</v>
       </c>
@@ -4709,8 +6540,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q53">
+        <v>2.5</v>
+      </c>
+      <c r="R53">
+        <v>5</v>
+      </c>
+      <c r="S53">
+        <v>1</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="V53">
+        <f t="shared" si="4"/>
+        <v>250000</v>
+      </c>
+      <c r="W53">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2.6</v>
       </c>
@@ -4751,8 +6602,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q54">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="R54">
+        <v>5</v>
+      </c>
+      <c r="S54">
+        <v>1</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <f t="shared" si="4"/>
+        <v>254999.99999999997</v>
+      </c>
+      <c r="W54">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2.65</v>
       </c>
@@ -4793,8 +6664,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q55">
+        <v>2.6</v>
+      </c>
+      <c r="R55">
+        <v>5</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="V55">
+        <f t="shared" si="4"/>
+        <v>260000</v>
+      </c>
+      <c r="W55">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2.7</v>
       </c>
@@ -4835,8 +6726,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q56">
+        <v>2.65</v>
+      </c>
+      <c r="R56">
+        <v>5</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="T56">
+        <v>0</v>
+      </c>
+      <c r="V56">
+        <f t="shared" si="4"/>
+        <v>265000</v>
+      </c>
+      <c r="W56">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2.75</v>
       </c>
@@ -4877,8 +6788,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q57">
+        <v>2.7</v>
+      </c>
+      <c r="R57">
+        <v>5</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>0</v>
+      </c>
+      <c r="V57">
+        <f t="shared" si="4"/>
+        <v>270000</v>
+      </c>
+      <c r="W57">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2.8</v>
       </c>
@@ -4919,8 +6850,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q58">
+        <v>2.75</v>
+      </c>
+      <c r="R58">
+        <v>5</v>
+      </c>
+      <c r="S58">
+        <v>1</v>
+      </c>
+      <c r="T58">
+        <v>0</v>
+      </c>
+      <c r="V58">
+        <f t="shared" si="4"/>
+        <v>275000</v>
+      </c>
+      <c r="W58">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2.85</v>
       </c>
@@ -4961,8 +6912,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q59">
+        <v>2.8</v>
+      </c>
+      <c r="R59">
+        <v>5</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="V59">
+        <f t="shared" si="4"/>
+        <v>280000</v>
+      </c>
+      <c r="W59">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2.9</v>
       </c>
@@ -5003,8 +6974,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q60">
+        <v>2.85</v>
+      </c>
+      <c r="R60">
+        <v>5</v>
+      </c>
+      <c r="S60">
+        <v>1</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="V60">
+        <f t="shared" si="4"/>
+        <v>285000</v>
+      </c>
+      <c r="W60">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2.95</v>
       </c>
@@ -5045,8 +7036,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q61">
+        <v>2.9</v>
+      </c>
+      <c r="R61">
+        <v>5</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="V61">
+        <f t="shared" si="4"/>
+        <v>290000</v>
+      </c>
+      <c r="W61">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3</v>
       </c>
@@ -5087,8 +7098,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q62">
+        <v>2.95</v>
+      </c>
+      <c r="R62">
+        <v>5</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="T62">
+        <v>0</v>
+      </c>
+      <c r="V62">
+        <f t="shared" si="4"/>
+        <v>295000</v>
+      </c>
+      <c r="W62">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3.05</v>
       </c>
@@ -5129,8 +7160,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <v>3</v>
+      </c>
+      <c r="R63">
+        <v>5</v>
+      </c>
+      <c r="S63">
+        <v>1</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="V63">
+        <f t="shared" si="4"/>
+        <v>300000</v>
+      </c>
+      <c r="W63">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3.1</v>
       </c>
@@ -5171,8 +7222,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q64">
+        <v>3.05</v>
+      </c>
+      <c r="R64">
+        <v>5</v>
+      </c>
+      <c r="S64">
+        <v>1</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="V64">
+        <f t="shared" si="4"/>
+        <v>305000</v>
+      </c>
+      <c r="W64">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3.15</v>
       </c>
@@ -5213,8 +7284,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q65">
+        <v>3.1</v>
+      </c>
+      <c r="R65">
+        <v>5</v>
+      </c>
+      <c r="S65">
+        <v>1</v>
+      </c>
+      <c r="T65">
+        <v>0</v>
+      </c>
+      <c r="V65">
+        <f t="shared" si="4"/>
+        <v>310000</v>
+      </c>
+      <c r="W65">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3.2</v>
       </c>
@@ -5255,8 +7346,28 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <v>3.15</v>
+      </c>
+      <c r="R66">
+        <v>5</v>
+      </c>
+      <c r="S66">
+        <v>1</v>
+      </c>
+      <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="V66">
+        <f t="shared" si="4"/>
+        <v>315000</v>
+      </c>
+      <c r="W66">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3.25</v>
       </c>
@@ -5270,11 +7381,11 @@
         <v>-1</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F101" si="4">A67*10^(B67)</f>
+        <f t="shared" ref="F67:F101" si="6">A67*10^(B67)</f>
         <v>325000</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G101" si="5">C67*10^(D67)</f>
+        <f t="shared" ref="G67:G101" si="7">C67*10^(D67)</f>
         <v>0.98224</v>
       </c>
       <c r="I67">
@@ -5290,15 +7401,35 @@
         <v>0</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N102" si="6">I67*10^(J67)</f>
+        <f t="shared" ref="N67:N102" si="8">I67*10^(J67)</f>
         <v>65000</v>
       </c>
       <c r="O67">
-        <f t="shared" ref="O67:O102" si="7">K67*10^(L67)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="O67:O102" si="9">K67*10^(L67)</f>
+        <v>1</v>
+      </c>
+      <c r="Q67">
+        <v>3.2</v>
+      </c>
+      <c r="R67">
+        <v>5</v>
+      </c>
+      <c r="S67">
+        <v>1</v>
+      </c>
+      <c r="T67">
+        <v>0</v>
+      </c>
+      <c r="V67">
+        <f t="shared" si="4"/>
+        <v>320000</v>
+      </c>
+      <c r="W67">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3.3</v>
       </c>
@@ -5312,11 +7443,11 @@
         <v>-1</v>
       </c>
       <c r="F68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>330000</v>
       </c>
       <c r="G68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98330000000000006</v>
       </c>
       <c r="I68">
@@ -5332,15 +7463,35 @@
         <v>0</v>
       </c>
       <c r="N68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>66000</v>
       </c>
       <c r="O68">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q68">
+        <v>3.25</v>
+      </c>
+      <c r="R68">
+        <v>5</v>
+      </c>
+      <c r="S68">
+        <v>1</v>
+      </c>
+      <c r="T68">
+        <v>0</v>
+      </c>
+      <c r="V68">
+        <f t="shared" ref="V68:V102" si="10">Q68*10^(R68)</f>
+        <v>325000</v>
+      </c>
+      <c r="W68">
+        <f t="shared" ref="W68:W102" si="11">S68*10^(T68)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3.35</v>
       </c>
@@ -5354,11 +7505,11 @@
         <v>-1</v>
       </c>
       <c r="F69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>335000</v>
       </c>
       <c r="G69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98431000000000002</v>
       </c>
       <c r="I69">
@@ -5374,15 +7525,35 @@
         <v>0</v>
       </c>
       <c r="N69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>67000</v>
       </c>
       <c r="O69">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>3.3</v>
+      </c>
+      <c r="R69">
+        <v>5</v>
+      </c>
+      <c r="S69">
+        <v>1</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="V69">
+        <f t="shared" si="10"/>
+        <v>330000</v>
+      </c>
+      <c r="W69">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3.4</v>
       </c>
@@ -5396,11 +7567,11 @@
         <v>-1</v>
       </c>
       <c r="F70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>340000</v>
       </c>
       <c r="G70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98524999999999996</v>
       </c>
       <c r="I70">
@@ -5416,15 +7587,35 @@
         <v>0</v>
       </c>
       <c r="N70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>68000</v>
       </c>
       <c r="O70">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <v>3.35</v>
+      </c>
+      <c r="R70">
+        <v>5</v>
+      </c>
+      <c r="S70">
+        <v>1</v>
+      </c>
+      <c r="T70">
+        <v>0</v>
+      </c>
+      <c r="V70">
+        <f t="shared" si="10"/>
+        <v>335000</v>
+      </c>
+      <c r="W70">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3.45</v>
       </c>
@@ -5438,11 +7629,11 @@
         <v>-1</v>
       </c>
       <c r="F71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>345000</v>
       </c>
       <c r="G71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98614000000000002</v>
       </c>
       <c r="I71">
@@ -5458,15 +7649,35 @@
         <v>0</v>
       </c>
       <c r="N71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>69000</v>
       </c>
       <c r="O71">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <v>3.4</v>
+      </c>
+      <c r="R71">
+        <v>5</v>
+      </c>
+      <c r="S71">
+        <v>1</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <f t="shared" si="10"/>
+        <v>340000</v>
+      </c>
+      <c r="W71">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3.5</v>
       </c>
@@ -5480,11 +7691,11 @@
         <v>-1</v>
       </c>
       <c r="F72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>350000</v>
       </c>
       <c r="G72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98697000000000001</v>
       </c>
       <c r="I72">
@@ -5500,15 +7711,35 @@
         <v>0</v>
       </c>
       <c r="N72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>70000</v>
       </c>
       <c r="O72">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q72">
+        <v>3.45</v>
+      </c>
+      <c r="R72">
+        <v>5</v>
+      </c>
+      <c r="S72">
+        <v>1</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <f t="shared" si="10"/>
+        <v>345000</v>
+      </c>
+      <c r="W72">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3.55</v>
       </c>
@@ -5522,11 +7753,11 @@
         <v>-1</v>
       </c>
       <c r="F73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>355000</v>
       </c>
       <c r="G73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98775999999999997</v>
       </c>
       <c r="I73">
@@ -5542,15 +7773,35 @@
         <v>0</v>
       </c>
       <c r="N73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>71000</v>
       </c>
       <c r="O73">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q73">
+        <v>3.5</v>
+      </c>
+      <c r="R73">
+        <v>5</v>
+      </c>
+      <c r="S73">
+        <v>1</v>
+      </c>
+      <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="V73">
+        <f t="shared" si="10"/>
+        <v>350000</v>
+      </c>
+      <c r="W73">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3.6</v>
       </c>
@@ -5564,11 +7815,11 @@
         <v>-1</v>
       </c>
       <c r="F74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>360000</v>
       </c>
       <c r="G74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98849000000000009</v>
       </c>
       <c r="I74">
@@ -5584,15 +7835,35 @@
         <v>0</v>
       </c>
       <c r="N74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>72000</v>
       </c>
       <c r="O74">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q74">
+        <v>3.55</v>
+      </c>
+      <c r="R74">
+        <v>5</v>
+      </c>
+      <c r="S74">
+        <v>1</v>
+      </c>
+      <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="V74">
+        <f t="shared" si="10"/>
+        <v>355000</v>
+      </c>
+      <c r="W74">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3.65</v>
       </c>
@@ -5606,11 +7877,11 @@
         <v>-1</v>
       </c>
       <c r="F75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>365000</v>
       </c>
       <c r="G75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.98918000000000006</v>
       </c>
       <c r="I75">
@@ -5626,15 +7897,35 @@
         <v>0</v>
       </c>
       <c r="N75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>73000</v>
       </c>
       <c r="O75">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q75">
+        <v>3.6</v>
+      </c>
+      <c r="R75">
+        <v>5</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="V75">
+        <f t="shared" si="10"/>
+        <v>360000</v>
+      </c>
+      <c r="W75">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3.7</v>
       </c>
@@ -5648,11 +7939,11 @@
         <v>-1</v>
       </c>
       <c r="F76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>370000</v>
       </c>
       <c r="G76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.9898300000000001</v>
       </c>
       <c r="I76">
@@ -5668,15 +7959,35 @@
         <v>0</v>
       </c>
       <c r="N76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>74000</v>
       </c>
       <c r="O76">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q76">
+        <v>3.65</v>
+      </c>
+      <c r="R76">
+        <v>5</v>
+      </c>
+      <c r="S76">
+        <v>1</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="V76">
+        <f t="shared" si="10"/>
+        <v>365000</v>
+      </c>
+      <c r="W76">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3.75</v>
       </c>
@@ -5690,11 +8001,11 @@
         <v>-1</v>
       </c>
       <c r="F77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>375000</v>
       </c>
       <c r="G77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99045000000000005</v>
       </c>
       <c r="I77">
@@ -5710,15 +8021,35 @@
         <v>0</v>
       </c>
       <c r="N77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>75000</v>
       </c>
       <c r="O77">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q77">
+        <v>3.7</v>
+      </c>
+      <c r="R77">
+        <v>5</v>
+      </c>
+      <c r="S77">
+        <v>1</v>
+      </c>
+      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="V77">
+        <f t="shared" si="10"/>
+        <v>370000</v>
+      </c>
+      <c r="W77">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3.8</v>
       </c>
@@ -5732,11 +8063,11 @@
         <v>-1</v>
       </c>
       <c r="F78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>380000</v>
       </c>
       <c r="G78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99102000000000001</v>
       </c>
       <c r="I78">
@@ -5752,15 +8083,35 @@
         <v>0</v>
       </c>
       <c r="N78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>76000</v>
       </c>
       <c r="O78">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q78">
+        <v>3.75</v>
+      </c>
+      <c r="R78">
+        <v>5</v>
+      </c>
+      <c r="S78">
+        <v>1</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <f t="shared" si="10"/>
+        <v>375000</v>
+      </c>
+      <c r="W78">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>3.85</v>
       </c>
@@ -5774,11 +8125,11 @@
         <v>-1</v>
       </c>
       <c r="F79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>385000</v>
       </c>
       <c r="G79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99156</v>
       </c>
       <c r="I79">
@@ -5794,15 +8145,35 @@
         <v>0</v>
       </c>
       <c r="N79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>77000</v>
       </c>
       <c r="O79">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q79">
+        <v>3.8</v>
+      </c>
+      <c r="R79">
+        <v>5</v>
+      </c>
+      <c r="S79">
+        <v>1</v>
+      </c>
+      <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="V79">
+        <f t="shared" si="10"/>
+        <v>380000</v>
+      </c>
+      <c r="W79">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3.9</v>
       </c>
@@ -5816,11 +8187,11 @@
         <v>-1</v>
       </c>
       <c r="F80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>390000</v>
       </c>
       <c r="G80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99207000000000001</v>
       </c>
       <c r="I80">
@@ -5836,15 +8207,35 @@
         <v>0</v>
       </c>
       <c r="N80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>78000</v>
       </c>
       <c r="O80">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q80">
+        <v>3.85</v>
+      </c>
+      <c r="R80">
+        <v>5</v>
+      </c>
+      <c r="S80">
+        <v>1</v>
+      </c>
+      <c r="T80">
+        <v>0</v>
+      </c>
+      <c r="V80">
+        <f t="shared" si="10"/>
+        <v>385000</v>
+      </c>
+      <c r="W80">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3.95</v>
       </c>
@@ -5858,11 +8249,11 @@
         <v>-1</v>
       </c>
       <c r="F81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>395000</v>
       </c>
       <c r="G81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99255000000000004</v>
       </c>
       <c r="I81">
@@ -5878,15 +8269,35 @@
         <v>0</v>
       </c>
       <c r="N81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>79000</v>
       </c>
       <c r="O81">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q81">
+        <v>3.9</v>
+      </c>
+      <c r="R81">
+        <v>5</v>
+      </c>
+      <c r="S81">
+        <v>1</v>
+      </c>
+      <c r="T81">
+        <v>0</v>
+      </c>
+      <c r="V81">
+        <f t="shared" si="10"/>
+        <v>390000</v>
+      </c>
+      <c r="W81">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4</v>
       </c>
@@ -5900,11 +8311,11 @@
         <v>-1</v>
       </c>
       <c r="F82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>400000</v>
       </c>
       <c r="G82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99299000000000004</v>
       </c>
       <c r="I82">
@@ -5920,15 +8331,35 @@
         <v>0</v>
       </c>
       <c r="N82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80000</v>
       </c>
       <c r="O82">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q82">
+        <v>3.95</v>
+      </c>
+      <c r="R82">
+        <v>5</v>
+      </c>
+      <c r="S82">
+        <v>1</v>
+      </c>
+      <c r="T82">
+        <v>0</v>
+      </c>
+      <c r="V82">
+        <f t="shared" si="10"/>
+        <v>395000</v>
+      </c>
+      <c r="W82">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>4.05</v>
       </c>
@@ -5942,11 +8373,11 @@
         <v>-1</v>
       </c>
       <c r="F83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>405000</v>
       </c>
       <c r="G83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99342000000000008</v>
       </c>
       <c r="I83">
@@ -5962,15 +8393,35 @@
         <v>0</v>
       </c>
       <c r="N83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>81000</v>
       </c>
       <c r="O83">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q83">
+        <v>4</v>
+      </c>
+      <c r="R83">
+        <v>5</v>
+      </c>
+      <c r="S83">
+        <v>1</v>
+      </c>
+      <c r="T83">
+        <v>0</v>
+      </c>
+      <c r="V83">
+        <f t="shared" si="10"/>
+        <v>400000</v>
+      </c>
+      <c r="W83">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4.0999999999999996</v>
       </c>
@@ -5984,11 +8435,11 @@
         <v>-1</v>
       </c>
       <c r="F84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>409999.99999999994</v>
       </c>
       <c r="G84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99381000000000008</v>
       </c>
       <c r="I84">
@@ -6004,15 +8455,35 @@
         <v>0</v>
       </c>
       <c r="N84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>82000</v>
       </c>
       <c r="O84">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q84">
+        <v>4.05</v>
+      </c>
+      <c r="R84">
+        <v>5</v>
+      </c>
+      <c r="S84">
+        <v>1</v>
+      </c>
+      <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="V84">
+        <f t="shared" si="10"/>
+        <v>405000</v>
+      </c>
+      <c r="W84">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4.1500000000000004</v>
       </c>
@@ -6026,11 +8497,11 @@
         <v>-1</v>
       </c>
       <c r="F85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>415000.00000000006</v>
       </c>
       <c r="G85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99418000000000006</v>
       </c>
       <c r="I85">
@@ -6046,15 +8517,35 @@
         <v>0</v>
       </c>
       <c r="N85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>83000</v>
       </c>
       <c r="O85">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q85">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R85">
+        <v>5</v>
+      </c>
+      <c r="S85">
+        <v>1</v>
+      </c>
+      <c r="T85">
+        <v>0</v>
+      </c>
+      <c r="V85">
+        <f t="shared" si="10"/>
+        <v>409999.99999999994</v>
+      </c>
+      <c r="W85">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4.2</v>
       </c>
@@ -6068,11 +8559,11 @@
         <v>-1</v>
       </c>
       <c r="F86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>420000</v>
       </c>
       <c r="G86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99453000000000003</v>
       </c>
       <c r="I86">
@@ -6088,15 +8579,35 @@
         <v>0</v>
       </c>
       <c r="N86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>84000</v>
       </c>
       <c r="O86">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q86">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="R86">
+        <v>5</v>
+      </c>
+      <c r="S86">
+        <v>1</v>
+      </c>
+      <c r="T86">
+        <v>0</v>
+      </c>
+      <c r="V86">
+        <f t="shared" si="10"/>
+        <v>415000.00000000006</v>
+      </c>
+      <c r="W86">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4.25</v>
       </c>
@@ -6110,11 +8621,11 @@
         <v>-1</v>
       </c>
       <c r="F87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>425000</v>
       </c>
       <c r="G87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99486000000000008</v>
       </c>
       <c r="I87">
@@ -6130,15 +8641,35 @@
         <v>0</v>
       </c>
       <c r="N87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>85000</v>
       </c>
       <c r="O87">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q87">
+        <v>4.2</v>
+      </c>
+      <c r="R87">
+        <v>5</v>
+      </c>
+      <c r="S87">
+        <v>1</v>
+      </c>
+      <c r="T87">
+        <v>0</v>
+      </c>
+      <c r="V87">
+        <f t="shared" si="10"/>
+        <v>420000</v>
+      </c>
+      <c r="W87">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4.3</v>
       </c>
@@ -6152,11 +8683,11 @@
         <v>-1</v>
       </c>
       <c r="F88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>430000</v>
       </c>
       <c r="G88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99517000000000011</v>
       </c>
       <c r="I88">
@@ -6172,15 +8703,35 @@
         <v>0</v>
       </c>
       <c r="N88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>86000</v>
       </c>
       <c r="O88">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q88">
+        <v>4.25</v>
+      </c>
+      <c r="R88">
+        <v>5</v>
+      </c>
+      <c r="S88">
+        <v>1</v>
+      </c>
+      <c r="T88">
+        <v>0</v>
+      </c>
+      <c r="V88">
+        <f t="shared" si="10"/>
+        <v>425000</v>
+      </c>
+      <c r="W88">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4.3499999999999996</v>
       </c>
@@ -6194,11 +8745,11 @@
         <v>-1</v>
       </c>
       <c r="F89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>434999.99999999994</v>
       </c>
       <c r="G89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99546000000000001</v>
       </c>
       <c r="I89">
@@ -6214,15 +8765,35 @@
         <v>0</v>
       </c>
       <c r="N89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>87000</v>
       </c>
       <c r="O89">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q89">
+        <v>4.3</v>
+      </c>
+      <c r="R89">
+        <v>5</v>
+      </c>
+      <c r="S89">
+        <v>1</v>
+      </c>
+      <c r="T89">
+        <v>0</v>
+      </c>
+      <c r="V89">
+        <f t="shared" si="10"/>
+        <v>430000</v>
+      </c>
+      <c r="W89">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>4.4000000000000004</v>
       </c>
@@ -6236,11 +8807,11 @@
         <v>-1</v>
       </c>
       <c r="F90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>440000.00000000006</v>
       </c>
       <c r="G90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99573</v>
       </c>
       <c r="I90">
@@ -6256,15 +8827,35 @@
         <v>0</v>
       </c>
       <c r="N90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>88000</v>
       </c>
       <c r="O90">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q90">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="R90">
+        <v>5</v>
+      </c>
+      <c r="S90">
+        <v>1</v>
+      </c>
+      <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="V90">
+        <f t="shared" si="10"/>
+        <v>434999.99999999994</v>
+      </c>
+      <c r="W90">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4.45</v>
       </c>
@@ -6278,11 +8869,11 @@
         <v>-1</v>
       </c>
       <c r="F91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>445000</v>
       </c>
       <c r="G91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99598999999999993</v>
       </c>
       <c r="I91">
@@ -6298,15 +8889,35 @@
         <v>0</v>
       </c>
       <c r="N91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>89000</v>
       </c>
       <c r="O91">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q91">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R91">
+        <v>5</v>
+      </c>
+      <c r="S91">
+        <v>1</v>
+      </c>
+      <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="V91">
+        <f t="shared" si="10"/>
+        <v>440000.00000000006</v>
+      </c>
+      <c r="W91">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4.5</v>
       </c>
@@ -6320,11 +8931,11 @@
         <v>-1</v>
       </c>
       <c r="F92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>450000</v>
       </c>
       <c r="G92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99623000000000017</v>
       </c>
       <c r="I92">
@@ -6340,15 +8951,35 @@
         <v>0</v>
       </c>
       <c r="N92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>90000</v>
       </c>
       <c r="O92">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q92">
+        <v>4.45</v>
+      </c>
+      <c r="R92">
+        <v>5</v>
+      </c>
+      <c r="S92">
+        <v>1</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <f t="shared" si="10"/>
+        <v>445000</v>
+      </c>
+      <c r="W92">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>4.55</v>
       </c>
@@ -6362,11 +8993,11 @@
         <v>-1</v>
       </c>
       <c r="F93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>455000</v>
       </c>
       <c r="G93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99646000000000012</v>
       </c>
       <c r="I93">
@@ -6382,15 +9013,35 @@
         <v>0</v>
       </c>
       <c r="N93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>91000</v>
       </c>
       <c r="O93">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q93">
+        <v>4.5</v>
+      </c>
+      <c r="R93">
+        <v>5</v>
+      </c>
+      <c r="S93">
+        <v>1</v>
+      </c>
+      <c r="T93">
+        <v>0</v>
+      </c>
+      <c r="V93">
+        <f t="shared" si="10"/>
+        <v>450000</v>
+      </c>
+      <c r="W93">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>4.5999999999999996</v>
       </c>
@@ -6404,11 +9055,11 @@
         <v>-1</v>
       </c>
       <c r="F94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>459999.99999999994</v>
       </c>
       <c r="G94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99666999999999994</v>
       </c>
       <c r="I94">
@@ -6424,15 +9075,35 @@
         <v>0</v>
       </c>
       <c r="N94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>92000</v>
       </c>
       <c r="O94">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q94">
+        <v>4.55</v>
+      </c>
+      <c r="R94">
+        <v>5</v>
+      </c>
+      <c r="S94">
+        <v>1</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="V94">
+        <f t="shared" si="10"/>
+        <v>455000</v>
+      </c>
+      <c r="W94">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>4.6500000000000004</v>
       </c>
@@ -6446,11 +9117,11 @@
         <v>-1</v>
       </c>
       <c r="F95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>465000.00000000006</v>
       </c>
       <c r="G95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99687000000000003</v>
       </c>
       <c r="I95">
@@ -6466,15 +9137,35 @@
         <v>0</v>
       </c>
       <c r="N95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>93000</v>
       </c>
       <c r="O95">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q95">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R95">
+        <v>5</v>
+      </c>
+      <c r="S95">
+        <v>1</v>
+      </c>
+      <c r="T95">
+        <v>0</v>
+      </c>
+      <c r="V95">
+        <f t="shared" si="10"/>
+        <v>459999.99999999994</v>
+      </c>
+      <c r="W95">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4.7</v>
       </c>
@@ -6488,11 +9179,11 @@
         <v>-1</v>
       </c>
       <c r="F96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>470000</v>
       </c>
       <c r="G96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99705999999999995</v>
       </c>
       <c r="I96">
@@ -6508,15 +9199,35 @@
         <v>0</v>
       </c>
       <c r="N96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>94000</v>
       </c>
       <c r="O96">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q96">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="R96">
+        <v>5</v>
+      </c>
+      <c r="S96">
+        <v>1</v>
+      </c>
+      <c r="T96">
+        <v>0</v>
+      </c>
+      <c r="V96">
+        <f t="shared" si="10"/>
+        <v>465000.00000000006</v>
+      </c>
+      <c r="W96">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4.75</v>
       </c>
@@ -6530,11 +9241,11 @@
         <v>-1</v>
       </c>
       <c r="F97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>475000</v>
       </c>
       <c r="G97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99724000000000013</v>
       </c>
       <c r="I97">
@@ -6550,15 +9261,35 @@
         <v>0</v>
       </c>
       <c r="N97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>95000</v>
       </c>
       <c r="O97">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q97">
+        <v>4.7</v>
+      </c>
+      <c r="R97">
+        <v>5</v>
+      </c>
+      <c r="S97">
+        <v>1</v>
+      </c>
+      <c r="T97">
+        <v>0</v>
+      </c>
+      <c r="V97">
+        <f t="shared" si="10"/>
+        <v>470000</v>
+      </c>
+      <c r="W97">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>4.8</v>
       </c>
@@ -6572,11 +9303,11 @@
         <v>-1</v>
       </c>
       <c r="F98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>480000</v>
       </c>
       <c r="G98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99740000000000006</v>
       </c>
       <c r="I98">
@@ -6592,15 +9323,35 @@
         <v>0</v>
       </c>
       <c r="N98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>96000</v>
       </c>
       <c r="O98">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q98">
+        <v>4.75</v>
+      </c>
+      <c r="R98">
+        <v>5</v>
+      </c>
+      <c r="S98">
+        <v>1</v>
+      </c>
+      <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="V98">
+        <f t="shared" si="10"/>
+        <v>475000</v>
+      </c>
+      <c r="W98">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>4.8499999999999996</v>
       </c>
@@ -6614,11 +9365,11 @@
         <v>-1</v>
       </c>
       <c r="F99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>484999.99999999994</v>
       </c>
       <c r="G99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99756</v>
       </c>
       <c r="I99">
@@ -6634,15 +9385,35 @@
         <v>0</v>
       </c>
       <c r="N99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97000</v>
       </c>
       <c r="O99">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q99">
+        <v>4.8</v>
+      </c>
+      <c r="R99">
+        <v>5</v>
+      </c>
+      <c r="S99">
+        <v>1</v>
+      </c>
+      <c r="T99">
+        <v>0</v>
+      </c>
+      <c r="V99">
+        <f t="shared" si="10"/>
+        <v>480000</v>
+      </c>
+      <c r="W99">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>4.9000000000000004</v>
       </c>
@@ -6656,11 +9427,11 @@
         <v>-1</v>
       </c>
       <c r="F100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>490000.00000000006</v>
       </c>
       <c r="G100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.9977100000000001</v>
       </c>
       <c r="I100">
@@ -6676,15 +9447,35 @@
         <v>0</v>
       </c>
       <c r="N100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>98000</v>
       </c>
       <c r="O100">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q100">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="R100">
+        <v>5</v>
+      </c>
+      <c r="S100">
+        <v>1</v>
+      </c>
+      <c r="T100">
+        <v>0</v>
+      </c>
+      <c r="V100">
+        <f t="shared" si="10"/>
+        <v>484999.99999999994</v>
+      </c>
+      <c r="W100">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4.95</v>
       </c>
@@ -6698,11 +9489,11 @@
         <v>-1</v>
       </c>
       <c r="F101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>495000</v>
       </c>
       <c r="G101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99784000000000006</v>
       </c>
       <c r="I101">
@@ -6718,15 +9509,35 @@
         <v>0</v>
       </c>
       <c r="N101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>99000</v>
       </c>
       <c r="O101">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q101">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R101">
+        <v>5</v>
+      </c>
+      <c r="S101">
+        <v>1</v>
+      </c>
+      <c r="T101">
+        <v>0</v>
+      </c>
+      <c r="V101">
+        <f t="shared" si="10"/>
+        <v>490000.00000000006</v>
+      </c>
+      <c r="W101">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I102">
         <v>1</v>
       </c>
@@ -6740,11 +9551,31 @@
         <v>0</v>
       </c>
       <c r="N102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>100000</v>
       </c>
       <c r="O102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q102">
+        <v>4.95</v>
+      </c>
+      <c r="R102">
+        <v>5</v>
+      </c>
+      <c r="S102">
+        <v>1</v>
+      </c>
+      <c r="T102">
+        <v>0</v>
+      </c>
+      <c r="V102">
+        <f t="shared" si="10"/>
+        <v>495000</v>
+      </c>
+      <c r="W102">
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>